<commit_message>
Aggiunta soluzione esatta FK_£/random30_180_2_1000_1_2 calcolata in 90 ore
</commit_message>
<xml_diff>
--- a/instances/MKP solutions.xlsx
+++ b/instances/MKP solutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\IdeaProjects\KernelSearchGolinoCottiBeatrice\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA0F46-93CA-43E2-82AD-3D5E7AA216A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104375ED-A07D-438B-BF8A-CA5C12BEEB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMALL" sheetId="11" r:id="rId1"/>
@@ -6494,7 +6494,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6504,19 +6517,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6807,35 +6807,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="10"/>
-    <col min="2" max="2" width="61" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="10"/>
+    <col min="1" max="1" width="11.5546875" style="4"/>
+    <col min="2" max="2" width="61" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:139" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="2:139" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
@@ -6845,7 +6845,7 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="EI3" s="10">
+      <c r="EI3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -10484,11 +10484,11 @@
       <c r="D2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
@@ -18218,11 +18218,11 @@
       <c r="D2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
@@ -23231,18 +23231,18 @@
       </c>
     </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B316" s="11" t="s">
+      <c r="B316" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="C316" s="11"/>
-      <c r="D316" s="11"/>
-      <c r="E316" s="11">
+      <c r="C316" s="5"/>
+      <c r="D316" s="5"/>
+      <c r="E316" s="5">
         <v>0</v>
       </c>
-      <c r="F316" s="11">
+      <c r="F316" s="5">
         <v>20945</v>
       </c>
-      <c r="G316" s="11">
+      <c r="G316" s="5">
         <v>20947</v>
       </c>
     </row>
@@ -25933,8 +25933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9D0552-08ED-44D2-AE96-8ACE55B4A4C4}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="G363" sqref="B363:G363"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25952,11 +25952,11 @@
       <c r="D2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
@@ -26309,18 +26309,18 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="5" t="s">
         <v>1168</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5">
         <v>0</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="5">
         <v>47911</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="5">
         <v>47966</v>
       </c>
     </row>
@@ -26469,18 +26469,18 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="5" t="s">
         <v>1178</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5">
         <v>0</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="5">
         <v>46700</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="5">
         <v>46713</v>
       </c>
     </row>
@@ -28885,18 +28885,18 @@
       </c>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B186" s="11" t="s">
+      <c r="B186" s="5" t="s">
         <v>1329</v>
       </c>
-      <c r="C186" s="11"/>
-      <c r="D186" s="11"/>
-      <c r="E186" s="11">
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5">
         <v>0</v>
       </c>
-      <c r="F186" s="11">
+      <c r="F186" s="5">
         <v>38822</v>
       </c>
-      <c r="G186" s="11">
+      <c r="G186" s="5">
         <v>38827</v>
       </c>
     </row>
@@ -29157,18 +29157,18 @@
       </c>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B203" s="11" t="s">
+      <c r="B203" s="5" t="s">
         <v>1346</v>
       </c>
-      <c r="C203" s="11"/>
-      <c r="D203" s="11"/>
-      <c r="E203" s="11">
+      <c r="C203" s="5"/>
+      <c r="D203" s="5"/>
+      <c r="E203" s="5">
         <v>0</v>
       </c>
-      <c r="F203" s="11">
+      <c r="F203" s="5">
         <v>42988</v>
       </c>
-      <c r="G203" s="11">
+      <c r="G203" s="5">
         <v>43004</v>
       </c>
     </row>
@@ -30453,18 +30453,18 @@
       </c>
     </row>
     <row r="284" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B284" s="11" t="s">
+      <c r="B284" s="5" t="s">
         <v>1427</v>
       </c>
-      <c r="C284" s="11"/>
-      <c r="D284" s="11"/>
-      <c r="E284" s="11">
+      <c r="C284" s="5"/>
+      <c r="D284" s="5"/>
+      <c r="E284" s="5">
         <v>0</v>
       </c>
-      <c r="F284" s="11">
+      <c r="F284" s="5">
         <v>36198</v>
       </c>
-      <c r="G284" s="11">
+      <c r="G284" s="5">
         <v>36201</v>
       </c>
     </row>
@@ -30629,18 +30629,18 @@
       </c>
     </row>
     <row r="295" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B295" s="11" t="s">
+      <c r="B295" s="5" t="s">
         <v>1438</v>
       </c>
-      <c r="C295" s="11"/>
-      <c r="D295" s="11"/>
-      <c r="E295" s="11">
+      <c r="C295" s="5"/>
+      <c r="D295" s="5"/>
+      <c r="E295" s="5">
         <v>0</v>
       </c>
-      <c r="F295" s="11">
+      <c r="F295" s="5">
         <v>37680</v>
       </c>
-      <c r="G295" s="11">
+      <c r="G295" s="5">
         <v>37681</v>
       </c>
     </row>
@@ -30981,18 +30981,18 @@
       </c>
     </row>
     <row r="317" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B317" s="11" t="s">
+      <c r="B317" s="5" t="s">
         <v>1460</v>
       </c>
-      <c r="C317" s="11"/>
-      <c r="D317" s="11"/>
-      <c r="E317" s="11">
+      <c r="C317" s="5"/>
+      <c r="D317" s="5"/>
+      <c r="E317" s="5">
         <v>0</v>
       </c>
-      <c r="F317" s="11">
+      <c r="F317" s="5">
         <v>52666</v>
       </c>
-      <c r="G317" s="11">
+      <c r="G317" s="5">
         <v>33756</v>
       </c>
     </row>
@@ -31717,18 +31717,18 @@
       </c>
     </row>
     <row r="363" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B363" s="11" t="s">
+      <c r="B363" s="5" t="s">
         <v>1506</v>
       </c>
-      <c r="C363" s="11"/>
-      <c r="D363" s="11"/>
-      <c r="E363" s="11">
+      <c r="C363" s="5"/>
+      <c r="D363" s="5"/>
+      <c r="E363" s="5">
         <v>0</v>
       </c>
-      <c r="F363" s="11">
+      <c r="F363" s="5">
         <v>68070</v>
       </c>
-      <c r="G363" s="11">
+      <c r="G363" s="5">
         <v>68125</v>
       </c>
     </row>
@@ -33660,6 +33660,7 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33667,7 +33668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1EBEC4-D610-4C6A-ADCB-85EDB48DC2AD}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
+    <sheetView topLeftCell="A417" workbookViewId="0">
       <selection activeCell="G358" sqref="B358:G361"/>
     </sheetView>
   </sheetViews>
@@ -33686,11 +33687,11 @@
       <c r="D2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
@@ -34091,18 +34092,18 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="5" t="s">
         <v>1731</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5">
         <v>0</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="5">
         <v>80459</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="5">
         <v>80483</v>
       </c>
     </row>
@@ -36267,18 +36268,18 @@
       </c>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B164" s="11" t="s">
+      <c r="B164" s="5" t="s">
         <v>1867</v>
       </c>
-      <c r="C164" s="11"/>
-      <c r="D164" s="11"/>
-      <c r="E164" s="11">
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5">
         <v>0</v>
       </c>
-      <c r="F164" s="11">
+      <c r="F164" s="5">
         <v>96925</v>
       </c>
-      <c r="G164" s="11">
+      <c r="G164" s="5">
         <v>97053</v>
       </c>
     </row>
@@ -36523,18 +36524,18 @@
       </c>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B180" s="11" t="s">
+      <c r="B180" s="5" t="s">
         <v>1883</v>
       </c>
-      <c r="C180" s="11"/>
-      <c r="D180" s="11"/>
-      <c r="E180" s="11">
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5">
         <v>0</v>
       </c>
-      <c r="F180" s="11">
+      <c r="F180" s="5">
         <v>95602</v>
       </c>
-      <c r="G180" s="11">
+      <c r="G180" s="5">
         <v>95792</v>
       </c>
     </row>
@@ -36555,18 +36556,18 @@
       </c>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B182" s="11" t="s">
+      <c r="B182" s="5" t="s">
         <v>1885</v>
       </c>
-      <c r="C182" s="11"/>
-      <c r="D182" s="11"/>
-      <c r="E182" s="11">
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5">
         <v>0</v>
       </c>
-      <c r="F182" s="11">
+      <c r="F182" s="5">
         <v>98998</v>
       </c>
-      <c r="G182" s="11">
+      <c r="G182" s="5">
         <v>99019</v>
       </c>
     </row>
@@ -36619,34 +36620,34 @@
       </c>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B186" s="11" t="s">
+      <c r="B186" s="5" t="s">
         <v>1889</v>
       </c>
-      <c r="C186" s="11"/>
-      <c r="D186" s="11"/>
-      <c r="E186" s="11">
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5">
         <v>0</v>
       </c>
-      <c r="F186" s="11">
+      <c r="F186" s="5">
         <v>66227</v>
       </c>
-      <c r="G186" s="11">
+      <c r="G186" s="5">
         <v>66260</v>
       </c>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B187" s="11" t="s">
+      <c r="B187" s="5" t="s">
         <v>1890</v>
       </c>
-      <c r="C187" s="11"/>
-      <c r="D187" s="11"/>
-      <c r="E187" s="11">
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5">
         <v>0</v>
       </c>
-      <c r="F187" s="11">
+      <c r="F187" s="5">
         <v>67855</v>
       </c>
-      <c r="G187" s="11">
+      <c r="G187" s="5">
         <v>67882</v>
       </c>
     </row>
@@ -36667,18 +36668,18 @@
       </c>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B189" s="11" t="s">
+      <c r="B189" s="5" t="s">
         <v>1892</v>
       </c>
-      <c r="C189" s="11"/>
-      <c r="D189" s="11"/>
-      <c r="E189" s="11">
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="5">
         <v>0</v>
       </c>
-      <c r="F189" s="11">
+      <c r="F189" s="5">
         <v>66224</v>
       </c>
-      <c r="G189" s="11">
+      <c r="G189" s="5">
         <v>66236</v>
       </c>
     </row>
@@ -36699,50 +36700,50 @@
       </c>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B191" s="11" t="s">
+      <c r="B191" s="5" t="s">
         <v>1894</v>
       </c>
-      <c r="C191" s="11"/>
-      <c r="D191" s="11"/>
-      <c r="E191" s="11">
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="5">
         <v>0</v>
       </c>
-      <c r="F191" s="11">
+      <c r="F191" s="5">
         <v>65600</v>
       </c>
-      <c r="G191" s="11">
+      <c r="G191" s="5">
         <v>65629</v>
       </c>
     </row>
     <row r="192" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B192" s="11" t="s">
+      <c r="B192" s="5" t="s">
         <v>1895</v>
       </c>
-      <c r="C192" s="11"/>
-      <c r="D192" s="11"/>
-      <c r="E192" s="11">
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5">
         <v>0</v>
       </c>
-      <c r="F192" s="11">
+      <c r="F192" s="5">
         <v>66601</v>
       </c>
-      <c r="G192" s="11">
+      <c r="G192" s="5">
         <v>66624</v>
       </c>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B193" s="11" t="s">
+      <c r="B193" s="5" t="s">
         <v>1896</v>
       </c>
-      <c r="C193" s="11"/>
-      <c r="D193" s="11"/>
-      <c r="E193" s="11">
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="5">
         <v>0</v>
       </c>
-      <c r="F193" s="11">
+      <c r="F193" s="5">
         <v>68325</v>
       </c>
-      <c r="G193" s="11">
+      <c r="G193" s="5">
         <v>68345</v>
       </c>
     </row>
@@ -36779,18 +36780,18 @@
       </c>
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B196" s="11" t="s">
+      <c r="B196" s="5" t="s">
         <v>1899</v>
       </c>
-      <c r="C196" s="11"/>
-      <c r="D196" s="11"/>
-      <c r="E196" s="11">
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5">
         <v>0</v>
       </c>
-      <c r="F196" s="11">
+      <c r="F196" s="5">
         <v>59252</v>
       </c>
-      <c r="G196" s="11">
+      <c r="G196" s="5">
         <v>59278</v>
       </c>
     </row>
@@ -36811,50 +36812,50 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B198" s="11" t="s">
+      <c r="B198" s="5" t="s">
         <v>1901</v>
       </c>
-      <c r="C198" s="11"/>
-      <c r="D198" s="11"/>
-      <c r="E198" s="11">
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="5">
         <v>0</v>
       </c>
-      <c r="F198" s="11">
+      <c r="F198" s="5">
         <v>66497</v>
       </c>
-      <c r="G198" s="11">
+      <c r="G198" s="5">
         <v>66529</v>
       </c>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B199" s="11" t="s">
+      <c r="B199" s="5" t="s">
         <v>1902</v>
       </c>
-      <c r="C199" s="11"/>
-      <c r="D199" s="11"/>
-      <c r="E199" s="11">
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="5">
         <v>0</v>
       </c>
-      <c r="F199" s="11">
+      <c r="F199" s="5">
         <v>71020</v>
       </c>
-      <c r="G199" s="11">
+      <c r="G199" s="5">
         <v>71041</v>
       </c>
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B200" s="11" t="s">
+      <c r="B200" s="5" t="s">
         <v>1903</v>
       </c>
-      <c r="C200" s="11"/>
-      <c r="D200" s="11"/>
-      <c r="E200" s="11">
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="E200" s="5">
         <v>0</v>
       </c>
-      <c r="F200" s="11">
+      <c r="F200" s="5">
         <v>69188</v>
       </c>
-      <c r="G200" s="11">
+      <c r="G200" s="5">
         <v>69203</v>
       </c>
     </row>
@@ -36875,18 +36876,18 @@
       </c>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B202" s="11" t="s">
+      <c r="B202" s="5" t="s">
         <v>1905</v>
       </c>
-      <c r="C202" s="11"/>
-      <c r="D202" s="11"/>
-      <c r="E202" s="11">
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
+      <c r="E202" s="5">
         <v>0</v>
       </c>
-      <c r="F202" s="11">
+      <c r="F202" s="5">
         <v>63344</v>
       </c>
-      <c r="G202" s="11">
+      <c r="G202" s="5">
         <v>63349</v>
       </c>
     </row>
@@ -36907,18 +36908,18 @@
       </c>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B204" s="11" t="s">
+      <c r="B204" s="5" t="s">
         <v>1907</v>
       </c>
-      <c r="C204" s="11"/>
-      <c r="D204" s="11"/>
-      <c r="E204" s="11">
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
+      <c r="E204" s="5">
         <v>0</v>
       </c>
-      <c r="F204" s="11">
+      <c r="F204" s="5">
         <v>64917</v>
       </c>
-      <c r="G204" s="11">
+      <c r="G204" s="5">
         <v>64956</v>
       </c>
     </row>
@@ -37051,34 +37052,34 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B213" s="11" t="s">
+      <c r="B213" s="5" t="s">
         <v>1916</v>
       </c>
-      <c r="C213" s="11"/>
-      <c r="D213" s="11"/>
-      <c r="E213" s="11">
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+      <c r="E213" s="5">
         <v>0</v>
       </c>
-      <c r="F213" s="11">
+      <c r="F213" s="5">
         <v>61428</v>
       </c>
-      <c r="G213" s="11">
+      <c r="G213" s="5">
         <v>61848</v>
       </c>
     </row>
     <row r="214" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B214" s="11" t="s">
+      <c r="B214" s="5" t="s">
         <v>1917</v>
       </c>
-      <c r="C214" s="11"/>
-      <c r="D214" s="11"/>
-      <c r="E214" s="11">
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
+      <c r="E214" s="5">
         <v>0</v>
       </c>
-      <c r="F214" s="11">
+      <c r="F214" s="5">
         <v>62296</v>
       </c>
-      <c r="G214" s="11">
+      <c r="G214" s="5">
         <v>62345</v>
       </c>
     </row>
@@ -37179,18 +37180,18 @@
       </c>
     </row>
     <row r="221" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B221" s="11" t="s">
+      <c r="B221" s="5" t="s">
         <v>1924</v>
       </c>
-      <c r="C221" s="11"/>
-      <c r="D221" s="11"/>
-      <c r="E221" s="11">
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+      <c r="E221" s="5">
         <v>0</v>
       </c>
-      <c r="F221" s="11">
+      <c r="F221" s="5">
         <v>59637</v>
       </c>
-      <c r="G221" s="11">
+      <c r="G221" s="5">
         <v>59648</v>
       </c>
     </row>
@@ -37547,34 +37548,34 @@
       </c>
     </row>
     <row r="244" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B244" s="11" t="s">
+      <c r="B244" s="5" t="s">
         <v>1947</v>
       </c>
-      <c r="C244" s="11"/>
-      <c r="D244" s="11"/>
-      <c r="E244" s="11">
+      <c r="C244" s="5"/>
+      <c r="D244" s="5"/>
+      <c r="E244" s="5">
         <v>0</v>
       </c>
-      <c r="F244" s="11">
+      <c r="F244" s="5">
         <v>93685</v>
       </c>
-      <c r="G244" s="11">
+      <c r="G244" s="5">
         <v>93686</v>
       </c>
     </row>
     <row r="245" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B245" s="11" t="s">
+      <c r="B245" s="5" t="s">
         <v>1948</v>
       </c>
-      <c r="C245" s="11"/>
-      <c r="D245" s="11"/>
-      <c r="E245" s="11">
+      <c r="C245" s="5"/>
+      <c r="D245" s="5"/>
+      <c r="E245" s="5">
         <v>0</v>
       </c>
-      <c r="F245" s="11">
+      <c r="F245" s="5">
         <v>90074</v>
       </c>
-      <c r="G245" s="11">
+      <c r="G245" s="5">
         <v>90190</v>
       </c>
     </row>
@@ -37819,18 +37820,18 @@
       </c>
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B261" s="11" t="s">
+      <c r="B261" s="5" t="s">
         <v>1964</v>
       </c>
-      <c r="C261" s="11"/>
-      <c r="D261" s="11"/>
-      <c r="E261" s="11">
+      <c r="C261" s="5"/>
+      <c r="D261" s="5"/>
+      <c r="E261" s="5">
         <v>0</v>
       </c>
-      <c r="F261" s="11">
+      <c r="F261" s="5">
         <v>93544</v>
       </c>
-      <c r="G261" s="11">
+      <c r="G261" s="5">
         <v>93551</v>
       </c>
     </row>
@@ -37851,18 +37852,18 @@
       </c>
     </row>
     <row r="263" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B263" s="11" t="s">
+      <c r="B263" s="5" t="s">
         <v>1966</v>
       </c>
-      <c r="C263" s="11"/>
-      <c r="D263" s="11"/>
-      <c r="E263" s="11">
+      <c r="C263" s="5"/>
+      <c r="D263" s="5"/>
+      <c r="E263" s="5">
         <v>0</v>
       </c>
-      <c r="F263" s="11">
+      <c r="F263" s="5">
         <v>92465</v>
       </c>
-      <c r="G263" s="11">
+      <c r="G263" s="5">
         <v>92494</v>
       </c>
     </row>
@@ -37915,34 +37916,34 @@
       </c>
     </row>
     <row r="267" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B267" s="11" t="s">
+      <c r="B267" s="5" t="s">
         <v>1970</v>
       </c>
-      <c r="C267" s="11"/>
-      <c r="D267" s="11"/>
-      <c r="E267" s="11">
+      <c r="C267" s="5"/>
+      <c r="D267" s="5"/>
+      <c r="E267" s="5">
         <v>0</v>
       </c>
-      <c r="F267" s="11">
+      <c r="F267" s="5">
         <v>62206</v>
       </c>
-      <c r="G267" s="11">
+      <c r="G267" s="5">
         <v>62210</v>
       </c>
     </row>
     <row r="268" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B268" s="11" t="s">
+      <c r="B268" s="5" t="s">
         <v>1971</v>
       </c>
-      <c r="C268" s="11"/>
-      <c r="D268" s="11"/>
-      <c r="E268" s="11">
+      <c r="C268" s="5"/>
+      <c r="D268" s="5"/>
+      <c r="E268" s="5">
         <v>0</v>
       </c>
-      <c r="F268" s="11">
+      <c r="F268" s="5">
         <v>58514</v>
       </c>
-      <c r="G268" s="11">
+      <c r="G268" s="5">
         <v>58516</v>
       </c>
     </row>
@@ -38059,34 +38060,34 @@
       </c>
     </row>
     <row r="276" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B276" s="11" t="s">
+      <c r="B276" s="5" t="s">
         <v>1979</v>
       </c>
-      <c r="C276" s="11"/>
-      <c r="D276" s="11"/>
-      <c r="E276" s="11">
+      <c r="C276" s="5"/>
+      <c r="D276" s="5"/>
+      <c r="E276" s="5">
         <v>0</v>
       </c>
-      <c r="F276" s="11">
+      <c r="F276" s="5">
         <v>63087</v>
       </c>
-      <c r="G276" s="11">
+      <c r="G276" s="5">
         <v>63108</v>
       </c>
     </row>
     <row r="277" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B277" s="11" t="s">
+      <c r="B277" s="5" t="s">
         <v>1980</v>
       </c>
-      <c r="C277" s="11"/>
-      <c r="D277" s="11"/>
-      <c r="E277" s="11">
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+      <c r="E277" s="5">
         <v>0</v>
       </c>
-      <c r="F277" s="11">
+      <c r="F277" s="5">
         <v>59572</v>
       </c>
-      <c r="G277" s="11">
+      <c r="G277" s="5">
         <v>59581</v>
       </c>
     </row>
@@ -38123,18 +38124,18 @@
       </c>
     </row>
     <row r="280" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B280" s="11" t="s">
+      <c r="B280" s="5" t="s">
         <v>1983</v>
       </c>
-      <c r="C280" s="11"/>
-      <c r="D280" s="11"/>
-      <c r="E280" s="11">
+      <c r="C280" s="5"/>
+      <c r="D280" s="5"/>
+      <c r="E280" s="5">
         <v>0</v>
       </c>
-      <c r="F280" s="11">
+      <c r="F280" s="5">
         <v>62773</v>
       </c>
-      <c r="G280" s="11">
+      <c r="G280" s="5">
         <v>62792</v>
       </c>
     </row>
@@ -38187,18 +38188,18 @@
       </c>
     </row>
     <row r="284" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B284" s="11" t="s">
+      <c r="B284" s="5" t="s">
         <v>1987</v>
       </c>
-      <c r="C284" s="11"/>
-      <c r="D284" s="11"/>
-      <c r="E284" s="11">
+      <c r="C284" s="5"/>
+      <c r="D284" s="5"/>
+      <c r="E284" s="5">
         <v>0</v>
       </c>
-      <c r="F284" s="11">
+      <c r="F284" s="5">
         <v>59835</v>
       </c>
-      <c r="G284" s="11">
+      <c r="G284" s="5">
         <v>59921</v>
       </c>
     </row>
@@ -38219,18 +38220,18 @@
       </c>
     </row>
     <row r="286" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B286" s="11" t="s">
+      <c r="B286" s="5" t="s">
         <v>1989</v>
       </c>
-      <c r="C286" s="11"/>
-      <c r="D286" s="11"/>
-      <c r="E286" s="11">
+      <c r="C286" s="5"/>
+      <c r="D286" s="5"/>
+      <c r="E286" s="5">
         <v>0</v>
       </c>
-      <c r="F286" s="11">
+      <c r="F286" s="5">
         <v>56816</v>
       </c>
-      <c r="G286" s="11">
+      <c r="G286" s="5">
         <v>56918</v>
       </c>
     </row>
@@ -38267,98 +38268,98 @@
       </c>
     </row>
     <row r="289" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B289" s="11" t="s">
+      <c r="B289" s="5" t="s">
         <v>1992</v>
       </c>
-      <c r="C289" s="11"/>
-      <c r="D289" s="11"/>
-      <c r="E289" s="11">
+      <c r="C289" s="5"/>
+      <c r="D289" s="5"/>
+      <c r="E289" s="5">
         <v>0</v>
       </c>
-      <c r="F289" s="11">
+      <c r="F289" s="5">
         <v>58014</v>
       </c>
-      <c r="G289" s="11">
+      <c r="G289" s="5">
         <v>58163</v>
       </c>
     </row>
     <row r="290" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B290" s="11" t="s">
+      <c r="B290" s="5" t="s">
         <v>1993</v>
       </c>
-      <c r="C290" s="11"/>
-      <c r="D290" s="11"/>
-      <c r="E290" s="11">
+      <c r="C290" s="5"/>
+      <c r="D290" s="5"/>
+      <c r="E290" s="5">
         <v>0</v>
       </c>
-      <c r="F290" s="11">
+      <c r="F290" s="5">
         <v>57027</v>
       </c>
-      <c r="G290" s="11">
+      <c r="G290" s="5">
         <v>57037</v>
       </c>
     </row>
     <row r="291" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B291" s="11" t="s">
+      <c r="B291" s="5" t="s">
         <v>1994</v>
       </c>
-      <c r="C291" s="11"/>
-      <c r="D291" s="11"/>
-      <c r="E291" s="11">
+      <c r="C291" s="5"/>
+      <c r="D291" s="5"/>
+      <c r="E291" s="5">
         <v>0</v>
       </c>
-      <c r="F291" s="11">
+      <c r="F291" s="5">
         <v>57908</v>
       </c>
-      <c r="G291" s="11">
+      <c r="G291" s="5">
         <v>57962</v>
       </c>
     </row>
     <row r="292" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B292" s="11" t="s">
+      <c r="B292" s="5" t="s">
         <v>1995</v>
       </c>
-      <c r="C292" s="11"/>
-      <c r="D292" s="11"/>
-      <c r="E292" s="11">
+      <c r="C292" s="5"/>
+      <c r="D292" s="5"/>
+      <c r="E292" s="5">
         <v>0</v>
       </c>
-      <c r="F292" s="11">
+      <c r="F292" s="5">
         <v>60524</v>
       </c>
-      <c r="G292" s="11">
+      <c r="G292" s="5">
         <v>60525</v>
       </c>
     </row>
     <row r="293" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B293" s="11" t="s">
+      <c r="B293" s="5" t="s">
         <v>1996</v>
       </c>
-      <c r="C293" s="11"/>
-      <c r="D293" s="11"/>
-      <c r="E293" s="11">
+      <c r="C293" s="5"/>
+      <c r="D293" s="5"/>
+      <c r="E293" s="5">
         <v>0</v>
       </c>
-      <c r="F293" s="11">
+      <c r="F293" s="5">
         <v>58120</v>
       </c>
-      <c r="G293" s="11">
+      <c r="G293" s="5">
         <v>58145</v>
       </c>
     </row>
     <row r="294" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B294" s="11" t="s">
+      <c r="B294" s="5" t="s">
         <v>1997</v>
       </c>
-      <c r="C294" s="11"/>
-      <c r="D294" s="11"/>
-      <c r="E294" s="11">
+      <c r="C294" s="5"/>
+      <c r="D294" s="5"/>
+      <c r="E294" s="5">
         <v>0</v>
       </c>
-      <c r="F294" s="11">
+      <c r="F294" s="5">
         <v>58266</v>
       </c>
-      <c r="G294" s="11">
+      <c r="G294" s="5">
         <v>58407</v>
       </c>
     </row>
@@ -38379,18 +38380,18 @@
       </c>
     </row>
     <row r="296" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B296" s="11" t="s">
+      <c r="B296" s="5" t="s">
         <v>1999</v>
       </c>
-      <c r="C296" s="11"/>
-      <c r="D296" s="11"/>
-      <c r="E296" s="11">
+      <c r="C296" s="5"/>
+      <c r="D296" s="5"/>
+      <c r="E296" s="5">
         <v>0</v>
       </c>
-      <c r="F296" s="11">
+      <c r="F296" s="5">
         <v>56532</v>
       </c>
-      <c r="G296" s="11">
+      <c r="G296" s="5">
         <v>56538</v>
       </c>
     </row>
@@ -38411,18 +38412,18 @@
       </c>
     </row>
     <row r="298" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B298" s="11" t="s">
+      <c r="B298" s="5" t="s">
         <v>2001</v>
       </c>
-      <c r="C298" s="11"/>
-      <c r="D298" s="11"/>
-      <c r="E298" s="11">
+      <c r="C298" s="5"/>
+      <c r="D298" s="5"/>
+      <c r="E298" s="5">
         <v>0</v>
       </c>
-      <c r="F298" s="11">
+      <c r="F298" s="5">
         <v>58167</v>
       </c>
-      <c r="G298" s="11">
+      <c r="G298" s="5">
         <v>58178</v>
       </c>
     </row>
@@ -38443,34 +38444,34 @@
       </c>
     </row>
     <row r="300" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B300" s="11" t="s">
+      <c r="B300" s="5" t="s">
         <v>2003</v>
       </c>
-      <c r="C300" s="11"/>
-      <c r="D300" s="11"/>
-      <c r="E300" s="11">
+      <c r="C300" s="5"/>
+      <c r="D300" s="5"/>
+      <c r="E300" s="5">
         <v>0</v>
       </c>
-      <c r="F300" s="11">
+      <c r="F300" s="5">
         <v>61998</v>
       </c>
-      <c r="G300" s="11">
+      <c r="G300" s="5">
         <v>62006</v>
       </c>
     </row>
     <row r="301" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B301" s="11" t="s">
+      <c r="B301" s="5" t="s">
         <v>2004</v>
       </c>
-      <c r="C301" s="11"/>
-      <c r="D301" s="11"/>
-      <c r="E301" s="11">
+      <c r="C301" s="5"/>
+      <c r="D301" s="5"/>
+      <c r="E301" s="5">
         <v>0</v>
       </c>
-      <c r="F301" s="11">
+      <c r="F301" s="5">
         <v>55992</v>
       </c>
-      <c r="G301" s="11">
+      <c r="G301" s="5">
         <v>55997</v>
       </c>
     </row>
@@ -38507,322 +38508,322 @@
       </c>
     </row>
     <row r="304" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B304" s="11" t="s">
+      <c r="B304" s="5" t="s">
         <v>2007</v>
       </c>
-      <c r="C304" s="11"/>
-      <c r="D304" s="11"/>
-      <c r="E304" s="11">
+      <c r="C304" s="5"/>
+      <c r="D304" s="5"/>
+      <c r="E304" s="5">
         <v>0</v>
       </c>
-      <c r="F304" s="11">
+      <c r="F304" s="5">
         <v>58344</v>
       </c>
-      <c r="G304" s="11">
+      <c r="G304" s="5">
         <v>58351</v>
       </c>
     </row>
     <row r="305" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B305" s="11" t="s">
+      <c r="B305" s="5" t="s">
         <v>2008</v>
       </c>
-      <c r="C305" s="11"/>
-      <c r="D305" s="11"/>
-      <c r="E305" s="11">
+      <c r="C305" s="5"/>
+      <c r="D305" s="5"/>
+      <c r="E305" s="5">
         <v>0</v>
       </c>
-      <c r="F305" s="11">
+      <c r="F305" s="5">
         <v>54531</v>
       </c>
-      <c r="G305" s="11">
+      <c r="G305" s="5">
         <v>54534</v>
       </c>
     </row>
     <row r="306" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B306" s="11" t="s">
+      <c r="B306" s="5" t="s">
         <v>2009</v>
       </c>
-      <c r="C306" s="11"/>
-      <c r="D306" s="11"/>
-      <c r="E306" s="11">
+      <c r="C306" s="5"/>
+      <c r="D306" s="5"/>
+      <c r="E306" s="5">
         <v>0</v>
       </c>
-      <c r="F306" s="11">
+      <c r="F306" s="5">
         <v>55267</v>
       </c>
-      <c r="G306" s="11">
+      <c r="G306" s="5">
         <v>55318</v>
       </c>
     </row>
     <row r="307" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B307" s="11" t="s">
+      <c r="B307" s="5" t="s">
         <v>2010</v>
       </c>
-      <c r="C307" s="11"/>
-      <c r="D307" s="11"/>
-      <c r="E307" s="11">
+      <c r="C307" s="5"/>
+      <c r="D307" s="5"/>
+      <c r="E307" s="5">
         <v>0</v>
       </c>
-      <c r="F307" s="11">
+      <c r="F307" s="5">
         <v>56339</v>
       </c>
-      <c r="G307" s="11">
+      <c r="G307" s="5">
         <v>56340</v>
       </c>
     </row>
     <row r="308" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B308" s="11" t="s">
+      <c r="B308" s="5" t="s">
         <v>2011</v>
       </c>
-      <c r="C308" s="11"/>
-      <c r="D308" s="11"/>
-      <c r="E308" s="11">
+      <c r="C308" s="5"/>
+      <c r="D308" s="5"/>
+      <c r="E308" s="5">
         <v>0</v>
       </c>
-      <c r="F308" s="11">
+      <c r="F308" s="5">
         <v>56183</v>
       </c>
-      <c r="G308" s="11">
+      <c r="G308" s="5">
         <v>56184</v>
       </c>
     </row>
     <row r="309" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B309" s="11" t="s">
+      <c r="B309" s="5" t="s">
         <v>2012</v>
       </c>
-      <c r="C309" s="11"/>
-      <c r="D309" s="11"/>
-      <c r="E309" s="11">
+      <c r="C309" s="5"/>
+      <c r="D309" s="5"/>
+      <c r="E309" s="5">
         <v>0</v>
       </c>
-      <c r="F309" s="11">
+      <c r="F309" s="5">
         <v>56575</v>
       </c>
-      <c r="G309" s="11">
+      <c r="G309" s="5">
         <v>56593</v>
       </c>
     </row>
     <row r="310" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B310" s="11" t="s">
+      <c r="B310" s="5" t="s">
         <v>2013</v>
       </c>
-      <c r="C310" s="11"/>
-      <c r="D310" s="11"/>
-      <c r="E310" s="11">
+      <c r="C310" s="5"/>
+      <c r="D310" s="5"/>
+      <c r="E310" s="5">
         <v>0</v>
       </c>
-      <c r="F310" s="11">
+      <c r="F310" s="5">
         <v>55438</v>
       </c>
-      <c r="G310" s="11">
+      <c r="G310" s="5">
         <v>55457</v>
       </c>
     </row>
     <row r="311" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B311" s="11" t="s">
+      <c r="B311" s="5" t="s">
         <v>2014</v>
       </c>
-      <c r="C311" s="11"/>
-      <c r="D311" s="11"/>
-      <c r="E311" s="11">
+      <c r="C311" s="5"/>
+      <c r="D311" s="5"/>
+      <c r="E311" s="5">
         <v>0</v>
       </c>
-      <c r="F311" s="11">
+      <c r="F311" s="5">
         <v>56365</v>
       </c>
-      <c r="G311" s="11">
+      <c r="G311" s="5">
         <v>56372</v>
       </c>
     </row>
     <row r="312" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B312" s="11" t="s">
+      <c r="B312" s="5" t="s">
         <v>2015</v>
       </c>
-      <c r="C312" s="11"/>
-      <c r="D312" s="11"/>
-      <c r="E312" s="11">
+      <c r="C312" s="5"/>
+      <c r="D312" s="5"/>
+      <c r="E312" s="5">
         <v>0</v>
       </c>
-      <c r="F312" s="11">
+      <c r="F312" s="5">
         <v>58974</v>
       </c>
-      <c r="G312" s="11">
+      <c r="G312" s="5">
         <v>58975</v>
       </c>
     </row>
     <row r="313" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B313" s="11" t="s">
+      <c r="B313" s="5" t="s">
         <v>2016</v>
       </c>
-      <c r="C313" s="11"/>
-      <c r="D313" s="11"/>
-      <c r="E313" s="11">
+      <c r="C313" s="5"/>
+      <c r="D313" s="5"/>
+      <c r="E313" s="5">
         <v>0</v>
       </c>
-      <c r="F313" s="11">
+      <c r="F313" s="5">
         <v>56511</v>
       </c>
-      <c r="G313" s="11">
+      <c r="G313" s="5">
         <v>56565</v>
       </c>
     </row>
     <row r="314" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B314" s="11" t="s">
+      <c r="B314" s="5" t="s">
         <v>2017</v>
       </c>
-      <c r="C314" s="11"/>
-      <c r="D314" s="11"/>
-      <c r="E314" s="11">
+      <c r="C314" s="5"/>
+      <c r="D314" s="5"/>
+      <c r="E314" s="5">
         <v>0</v>
       </c>
-      <c r="F314" s="11">
+      <c r="F314" s="5">
         <v>56790</v>
       </c>
-      <c r="G314" s="11">
+      <c r="G314" s="5">
         <v>56827</v>
       </c>
     </row>
     <row r="315" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B315" s="11" t="s">
+      <c r="B315" s="5" t="s">
         <v>2018</v>
       </c>
-      <c r="C315" s="11"/>
-      <c r="D315" s="11"/>
-      <c r="E315" s="11">
+      <c r="C315" s="5"/>
+      <c r="D315" s="5"/>
+      <c r="E315" s="5">
         <v>0</v>
       </c>
-      <c r="F315" s="11">
+      <c r="F315" s="5">
         <v>55708</v>
       </c>
-      <c r="G315" s="11">
+      <c r="G315" s="5">
         <v>55736</v>
       </c>
     </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B316" s="11" t="s">
+      <c r="B316" s="5" t="s">
         <v>2019</v>
       </c>
-      <c r="C316" s="11"/>
-      <c r="D316" s="11"/>
-      <c r="E316" s="11">
+      <c r="C316" s="5"/>
+      <c r="D316" s="5"/>
+      <c r="E316" s="5">
         <v>0</v>
       </c>
-      <c r="F316" s="11">
+      <c r="F316" s="5">
         <v>54946</v>
       </c>
-      <c r="G316" s="11">
+      <c r="G316" s="5">
         <v>54948</v>
       </c>
     </row>
     <row r="317" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B317" s="11" t="s">
+      <c r="B317" s="5" t="s">
         <v>2020</v>
       </c>
-      <c r="C317" s="11"/>
-      <c r="D317" s="11"/>
-      <c r="E317" s="11">
+      <c r="C317" s="5"/>
+      <c r="D317" s="5"/>
+      <c r="E317" s="5">
         <v>0</v>
       </c>
-      <c r="F317" s="11">
+      <c r="F317" s="5">
         <v>56425</v>
       </c>
-      <c r="G317" s="11">
+      <c r="G317" s="5">
         <v>56427</v>
       </c>
     </row>
     <row r="318" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B318" s="11" t="s">
+      <c r="B318" s="5" t="s">
         <v>2021</v>
       </c>
-      <c r="C318" s="11"/>
-      <c r="D318" s="11"/>
-      <c r="E318" s="11">
+      <c r="C318" s="5"/>
+      <c r="D318" s="5"/>
+      <c r="E318" s="5">
         <v>0</v>
       </c>
-      <c r="F318" s="11">
+      <c r="F318" s="5">
         <v>56593</v>
       </c>
-      <c r="G318" s="11">
+      <c r="G318" s="5">
         <v>56598</v>
       </c>
     </row>
     <row r="319" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B319" s="11" t="s">
+      <c r="B319" s="5" t="s">
         <v>2022</v>
       </c>
-      <c r="C319" s="11"/>
-      <c r="D319" s="11"/>
-      <c r="E319" s="11">
+      <c r="C319" s="5"/>
+      <c r="D319" s="5"/>
+      <c r="E319" s="5">
         <v>0</v>
       </c>
-      <c r="F319" s="11">
+      <c r="F319" s="5">
         <v>59535</v>
       </c>
-      <c r="G319" s="11">
+      <c r="G319" s="5">
         <v>59536</v>
       </c>
     </row>
     <row r="320" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B320" s="11" t="s">
+      <c r="B320" s="5" t="s">
         <v>2023</v>
       </c>
-      <c r="C320" s="11"/>
-      <c r="D320" s="11"/>
-      <c r="E320" s="11">
+      <c r="C320" s="5"/>
+      <c r="D320" s="5"/>
+      <c r="E320" s="5">
         <v>0</v>
       </c>
-      <c r="F320" s="11">
+      <c r="F320" s="5">
         <v>60456</v>
       </c>
-      <c r="G320" s="11">
+      <c r="G320" s="5">
         <v>60458</v>
       </c>
     </row>
     <row r="321" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B321" s="11" t="s">
+      <c r="B321" s="5" t="s">
         <v>2024</v>
       </c>
-      <c r="C321" s="11"/>
-      <c r="D321" s="11"/>
-      <c r="E321" s="11">
+      <c r="C321" s="5"/>
+      <c r="D321" s="5"/>
+      <c r="E321" s="5">
         <v>0</v>
       </c>
-      <c r="F321" s="11">
+      <c r="F321" s="5">
         <v>54411</v>
       </c>
-      <c r="G321" s="11">
+      <c r="G321" s="5">
         <v>54417</v>
       </c>
     </row>
     <row r="322" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B322" s="11" t="s">
+      <c r="B322" s="5" t="s">
         <v>2025</v>
       </c>
-      <c r="C322" s="11"/>
-      <c r="D322" s="11"/>
-      <c r="E322" s="11">
+      <c r="C322" s="5"/>
+      <c r="D322" s="5"/>
+      <c r="E322" s="5">
         <v>0</v>
       </c>
-      <c r="F322" s="11">
+      <c r="F322" s="5">
         <v>57339</v>
       </c>
-      <c r="G322" s="11">
+      <c r="G322" s="5">
         <v>57348</v>
       </c>
     </row>
     <row r="323" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B323" s="11" t="s">
+      <c r="B323" s="5" t="s">
         <v>2026</v>
       </c>
-      <c r="C323" s="11"/>
-      <c r="D323" s="11"/>
-      <c r="E323" s="11">
+      <c r="C323" s="5"/>
+      <c r="D323" s="5"/>
+      <c r="E323" s="5">
         <v>0</v>
       </c>
-      <c r="F323" s="11">
+      <c r="F323" s="5">
         <v>58338</v>
       </c>
-      <c r="G323" s="11">
+      <c r="G323" s="5">
         <v>58340</v>
       </c>
     </row>
@@ -39035,18 +39036,18 @@
       </c>
     </row>
     <row r="337" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B337" s="11" t="s">
+      <c r="B337" s="5" t="s">
         <v>2040</v>
       </c>
-      <c r="C337" s="11"/>
-      <c r="D337" s="11"/>
-      <c r="E337" s="11">
+      <c r="C337" s="5"/>
+      <c r="D337" s="5"/>
+      <c r="E337" s="5">
         <v>0</v>
       </c>
-      <c r="F337" s="11">
+      <c r="F337" s="5">
         <v>144487</v>
       </c>
-      <c r="G337" s="11">
+      <c r="G337" s="5">
         <v>144613</v>
       </c>
     </row>
@@ -39163,18 +39164,18 @@
       </c>
     </row>
     <row r="345" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B345" s="11" t="s">
+      <c r="B345" s="5" t="s">
         <v>2048</v>
       </c>
-      <c r="C345" s="11"/>
-      <c r="D345" s="11"/>
-      <c r="E345" s="11">
+      <c r="C345" s="5"/>
+      <c r="D345" s="5"/>
+      <c r="E345" s="5">
         <v>0</v>
       </c>
-      <c r="F345" s="11">
+      <c r="F345" s="5">
         <v>98324</v>
       </c>
-      <c r="G345" s="11">
+      <c r="G345" s="5">
         <v>98587</v>
       </c>
     </row>
@@ -39195,18 +39196,18 @@
       </c>
     </row>
     <row r="347" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B347" s="11" t="s">
+      <c r="B347" s="5" t="s">
         <v>2050</v>
       </c>
-      <c r="C347" s="11"/>
-      <c r="D347" s="11"/>
-      <c r="E347" s="11">
+      <c r="C347" s="5"/>
+      <c r="D347" s="5"/>
+      <c r="E347" s="5">
         <v>0</v>
       </c>
-      <c r="F347" s="11">
+      <c r="F347" s="5">
         <v>103025</v>
       </c>
-      <c r="G347" s="11">
+      <c r="G347" s="5">
         <v>99999</v>
       </c>
     </row>
@@ -39243,18 +39244,18 @@
       </c>
     </row>
     <row r="350" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B350" s="11" t="s">
+      <c r="B350" s="5" t="s">
         <v>2053</v>
       </c>
-      <c r="C350" s="11"/>
-      <c r="D350" s="11"/>
-      <c r="E350" s="11">
+      <c r="C350" s="5"/>
+      <c r="D350" s="5"/>
+      <c r="E350" s="5">
         <v>0</v>
       </c>
-      <c r="F350" s="11">
+      <c r="F350" s="5">
         <v>105438</v>
       </c>
-      <c r="G350" s="11">
+      <c r="G350" s="5">
         <v>99999</v>
       </c>
     </row>
@@ -39275,18 +39276,18 @@
       </c>
     </row>
     <row r="352" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B352" s="11" t="s">
+      <c r="B352" s="5" t="s">
         <v>2055</v>
       </c>
-      <c r="C352" s="11"/>
-      <c r="D352" s="11"/>
-      <c r="E352" s="11">
+      <c r="C352" s="5"/>
+      <c r="D352" s="5"/>
+      <c r="E352" s="5">
         <v>0</v>
       </c>
-      <c r="F352" s="11">
+      <c r="F352" s="5">
         <v>102761</v>
       </c>
-      <c r="G352" s="11">
+      <c r="G352" s="5">
         <v>102866</v>
       </c>
     </row>
@@ -39307,18 +39308,18 @@
       </c>
     </row>
     <row r="354" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B354" s="11" t="s">
+      <c r="B354" s="5" t="s">
         <v>2057</v>
       </c>
-      <c r="C354" s="11"/>
-      <c r="D354" s="11"/>
-      <c r="E354" s="11">
+      <c r="C354" s="5"/>
+      <c r="D354" s="5"/>
+      <c r="E354" s="5">
         <v>0</v>
       </c>
-      <c r="F354" s="11">
+      <c r="F354" s="5">
         <v>102695</v>
       </c>
-      <c r="G354" s="11">
+      <c r="G354" s="5">
         <v>99999</v>
       </c>
     </row>
@@ -39371,66 +39372,66 @@
       </c>
     </row>
     <row r="358" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B358" s="11" t="s">
+      <c r="B358" s="5" t="s">
         <v>2061</v>
       </c>
-      <c r="C358" s="11"/>
-      <c r="D358" s="11"/>
-      <c r="E358" s="11">
+      <c r="C358" s="5"/>
+      <c r="D358" s="5"/>
+      <c r="E358" s="5">
         <v>0</v>
       </c>
-      <c r="F358" s="11">
+      <c r="F358" s="5">
         <v>104468</v>
       </c>
-      <c r="G358" s="11">
+      <c r="G358" s="5">
         <v>99999</v>
       </c>
     </row>
     <row r="359" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B359" s="11" t="s">
+      <c r="B359" s="5" t="s">
         <v>2062</v>
       </c>
-      <c r="C359" s="11"/>
-      <c r="D359" s="11"/>
-      <c r="E359" s="11">
+      <c r="C359" s="5"/>
+      <c r="D359" s="5"/>
+      <c r="E359" s="5">
         <v>0</v>
       </c>
-      <c r="F359" s="11">
+      <c r="F359" s="5">
         <v>110182</v>
       </c>
-      <c r="G359" s="11">
+      <c r="G359" s="5">
         <v>99999</v>
       </c>
     </row>
     <row r="360" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B360" s="11" t="s">
+      <c r="B360" s="5" t="s">
         <v>2063</v>
       </c>
-      <c r="C360" s="11"/>
-      <c r="D360" s="11"/>
-      <c r="E360" s="11">
+      <c r="C360" s="5"/>
+      <c r="D360" s="5"/>
+      <c r="E360" s="5">
         <v>0</v>
       </c>
-      <c r="F360" s="11">
+      <c r="F360" s="5">
         <v>105542</v>
       </c>
-      <c r="G360" s="11">
+      <c r="G360" s="5">
         <v>99999</v>
       </c>
     </row>
     <row r="361" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B361" s="11" t="s">
+      <c r="B361" s="5" t="s">
         <v>2064</v>
       </c>
-      <c r="C361" s="11"/>
-      <c r="D361" s="11"/>
-      <c r="E361" s="11">
+      <c r="C361" s="5"/>
+      <c r="D361" s="5"/>
+      <c r="E361" s="5">
         <v>0</v>
       </c>
-      <c r="F361" s="11">
+      <c r="F361" s="5">
         <v>101942</v>
       </c>
-      <c r="G361" s="11">
+      <c r="G361" s="5">
         <v>99999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiunta della stampa del tempo totale d'esecuzione
</commit_message>
<xml_diff>
--- a/instances/MKP solutions.xlsx
+++ b/instances/MKP solutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\IdeaProjects\KernelSearchGolinoCottiBeatrice\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104375ED-A07D-438B-BF8A-CA5C12BEEB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CD40B2-7AB2-42FA-BEDB-1A319C59F281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMALL" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="2107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="2109">
   <si>
     <t>Instance</t>
   </si>
@@ -6359,6 +6359,12 @@
   </si>
   <si>
     <t>_OUTPUT/random75_375_4_1000_1_20.txt_MULKNAP_EASY.txt</t>
+  </si>
+  <si>
+    <t>Esatto</t>
+  </si>
+  <si>
+    <t>90H - 0,12% -47968.5962</t>
   </si>
 </sst>
 </file>
@@ -6801,7 +6807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A597B76-4812-4C27-9815-9F9D5B6A4480}">
   <dimension ref="B2:EI183"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E196" sqref="E196"/>
     </sheetView>
   </sheetViews>
@@ -10465,7 +10471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2288648E-97D4-4552-A3A6-9FF34DD9ED00}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A468" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E497" sqref="E497"/>
     </sheetView>
   </sheetViews>
@@ -18199,7 +18205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F45A19-6EEA-44AF-B354-43B8CAFCBABB}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A465" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E494" sqref="E494"/>
     </sheetView>
   </sheetViews>
@@ -25931,15 +25937,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9D0552-08ED-44D2-AE96-8ACE55B4A4C4}">
-  <dimension ref="B2:G483"/>
+  <dimension ref="B2:I483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="55.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
@@ -26180,7 +26187,7 @@
         <v>73606</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>1160</v>
       </c>
@@ -26196,7 +26203,7 @@
         <v>73648</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>1161</v>
       </c>
@@ -26212,7 +26219,7 @@
         <v>73127</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>1162</v>
       </c>
@@ -26228,7 +26235,7 @@
         <v>71606</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>1163</v>
       </c>
@@ -26244,7 +26251,7 @@
         <v>70663</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>1164</v>
       </c>
@@ -26260,7 +26267,7 @@
         <v>74218</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>1165</v>
       </c>
@@ -26276,7 +26283,7 @@
         <v>74016</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>1166</v>
       </c>
@@ -26292,7 +26299,7 @@
         <v>75618</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>1167</v>
       </c>
@@ -26307,8 +26314,11 @@
       <c r="G24" s="1">
         <v>52819</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>1168</v>
       </c>
@@ -26323,8 +26333,11 @@
       <c r="G25" s="5">
         <v>47966</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1169</v>
       </c>
@@ -26340,7 +26353,7 @@
         <v>50040</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>1170</v>
       </c>
@@ -26356,7 +26369,7 @@
         <v>50064</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>1171</v>
       </c>
@@ -26372,7 +26385,7 @@
         <v>50546</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>1172</v>
       </c>
@@ -26388,7 +26401,7 @@
         <v>48077</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>1173</v>
       </c>
@@ -26404,7 +26417,7 @@
         <v>50673</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>1174</v>
       </c>
@@ -26420,7 +26433,7 @@
         <v>49824</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>1175</v>
       </c>
@@ -33668,8 +33681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1EBEC4-D610-4C6A-ADCB-85EDB48DC2AD}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A417" workbookViewId="0">
-      <selection activeCell="G358" sqref="B358:G361"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Creazione del sorter per profitto/peso
</commit_message>
<xml_diff>
--- a/instances/MKP solutions.xlsx
+++ b/instances/MKP solutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\IdeaProjects\KernelSearchGolinoCottiBeatrice\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CD40B2-7AB2-42FA-BEDB-1A319C59F281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A82AC8-92A9-466D-8240-6FB32D30E4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMALL" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="2109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="2107">
   <si>
     <t>Instance</t>
   </si>
@@ -6359,12 +6359,6 @@
   </si>
   <si>
     <t>_OUTPUT/random75_375_4_1000_1_20.txt_MULKNAP_EASY.txt</t>
-  </si>
-  <si>
-    <t>Esatto</t>
-  </si>
-  <si>
-    <t>90H - 0,12% -47968.5962</t>
   </si>
 </sst>
 </file>
@@ -25937,10 +25931,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9D0552-08ED-44D2-AE96-8ACE55B4A4C4}">
-  <dimension ref="B2:I483"/>
+  <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26187,7 +26181,7 @@
         <v>73606</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>1160</v>
       </c>
@@ -26203,7 +26197,7 @@
         <v>73648</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>1161</v>
       </c>
@@ -26219,7 +26213,7 @@
         <v>73127</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>1162</v>
       </c>
@@ -26235,7 +26229,7 @@
         <v>71606</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>1163</v>
       </c>
@@ -26251,7 +26245,7 @@
         <v>70663</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>1164</v>
       </c>
@@ -26267,7 +26261,7 @@
         <v>74218</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>1165</v>
       </c>
@@ -26283,7 +26277,7 @@
         <v>74016</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>1166</v>
       </c>
@@ -26299,7 +26293,7 @@
         <v>75618</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>1167</v>
       </c>
@@ -26314,11 +26308,8 @@
       <c r="G24" s="1">
         <v>52819</v>
       </c>
-      <c r="I24" t="s">
-        <v>2107</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>1168</v>
       </c>
@@ -26333,11 +26324,8 @@
       <c r="G25" s="5">
         <v>47966</v>
       </c>
-      <c r="I25" t="s">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1169</v>
       </c>
@@ -26353,7 +26341,7 @@
         <v>50040</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>1170</v>
       </c>
@@ -26369,7 +26357,7 @@
         <v>50064</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>1171</v>
       </c>
@@ -26385,7 +26373,7 @@
         <v>50546</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>1172</v>
       </c>
@@ -26401,7 +26389,7 @@
         <v>48077</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>1173</v>
       </c>
@@ -26417,7 +26405,7 @@
         <v>50673</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>1174</v>
       </c>
@@ -26433,7 +26421,7 @@
         <v>49824</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>1175</v>
       </c>
@@ -33681,7 +33669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1EBEC4-D610-4C6A-ADCB-85EDB48DC2AD}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Selezione delle istanze di test Sono state selezionate 5 istanze risolte non all'ottimo per ogni cartella (se esistono)
</commit_message>
<xml_diff>
--- a/instances/MKP solutions.xlsx
+++ b/instances/MKP solutions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\IdeaProjects\KernelSearchGolinoCottiBeatrice\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A82AC8-92A9-466D-8240-6FB32D30E4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE254F85-F3A1-4070-8805-B02AEF969A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMALL" sheetId="11" r:id="rId1"/>
@@ -25933,8 +25933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9D0552-08ED-44D2-AE96-8ACE55B4A4C4}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33669,8 +33669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1EBEC4-D610-4C6A-ADCB-85EDB48DC2AD}">
   <dimension ref="B2:G483"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B323" sqref="B323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>